<commit_message>
Added queirks and stats for every one except ork
</commit_message>
<xml_diff>
--- a/dataBase/automatonAncestry.xlsx
+++ b/dataBase/automatonAncestry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24288010-012F-4706-866B-D53DEF7CA748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6660CE-3348-44F5-88FA-AA03C5A57691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="automatonAncestry" sheetId="1" r:id="rId1"/>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1C835C-BECA-4F8C-A233-A9EE9639DEEB}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1042,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>29</v>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1568,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A5E2F9-0AA5-4A58-B473-4820B5637D5F}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cleared up some of the code that was unnecessary
</commit_message>
<xml_diff>
--- a/dataBase/automatonAncestry.xlsx
+++ b/dataBase/automatonAncestry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6660CE-3348-44F5-88FA-AA03C5A57691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E60842-C63C-441F-A79A-4CC6A00CE61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1655,7 +1655,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding methods to add items to pdf with multidimentional tables
</commit_message>
<xml_diff>
--- a/dataBase/automatonAncestry.xlsx
+++ b/dataBase/automatonAncestry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E60842-C63C-441F-A79A-4CC6A00CE61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B66A014-31AF-4E88-AF92-D8DB5E6894A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="automatonAncestry" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="104">
   <si>
     <t>Wspólny</t>
   </si>
@@ -303,9 +303,6 @@
   <si>
     <t>Mały, człekopodobny automaton. Zmniejsz swój
 Rozmiar do 1/2. Masz około 120 centymetrów wzrostu i ważysz około 30 kilogramów.</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
   <si>
     <t>Człekopodobny automaton. Masz około 180 centymetrów wzrostu i ważysz około 150 kilogramów.</t>
@@ -1030,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1C835C-BECA-4F8C-A233-A9EE9639DEEB}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,9 +1100,6 @@
       </c>
       <c r="B7" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1595,7 +1589,7 @@
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>87</v>
@@ -1603,7 +1597,7 @@
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>88</v>
@@ -1611,10 +1605,10 @@
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1622,7 +1616,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -1630,7 +1624,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1654,7 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A5E2F9-0AA5-4A58-B473-4820B5637D5F}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1674,18 +1668,18 @@
     </row>
     <row r="2" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1693,23 +1687,23 @@
         <v>25</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>